<commit_message>
comit date: Jan 11,2021
</commit_message>
<xml_diff>
--- a/src/test/java/com/ccs/testData/LoginData.xlsx
+++ b/src/test/java/com/ccs/testData/LoginData.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="ContentData" sheetId="3" r:id="rId3"/>
     <sheet name="DocumentData" sheetId="4" r:id="rId4"/>
     <sheet name="LayoutData" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId6"/>
-    <sheet name="StyleData" sheetId="8" r:id="rId7"/>
+    <sheet name="StyleData" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
   <si>
     <t>username</t>
   </si>
@@ -82,30 +82,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>CC-BillingStatement2</t>
-  </si>
-  <si>
-    <t>CC-Billing Statement2</t>
-  </si>
-  <si>
-    <t>CC-BillingStatementV3</t>
-  </si>
-  <si>
-    <t>CC-BillingStatement  Version3</t>
-  </si>
-  <si>
-    <t>CC-BillingStatement6</t>
-  </si>
-  <si>
-    <t>CC-Billing Statement6</t>
-  </si>
-  <si>
-    <t>CC-BillingStatement6V1</t>
-  </si>
-  <si>
-    <t>CC-BillingStatement6 Version1</t>
-  </si>
-  <si>
     <t>BaseDocName</t>
   </si>
   <si>
@@ -151,9 +127,6 @@
     <t>SearchName</t>
   </si>
   <si>
-    <t>cc</t>
-  </si>
-  <si>
     <t>LayoutName</t>
   </si>
   <si>
@@ -205,21 +178,9 @@
     <t>uiiu</t>
   </si>
   <si>
-    <t>CC-SampleLayout5</t>
-  </si>
-  <si>
-    <t>CC-SampleLayout5 Longname</t>
-  </si>
-  <si>
     <t>CC</t>
   </si>
   <si>
-    <t>CC-SampleStyle</t>
-  </si>
-  <si>
-    <t>CC-SampleStyle Longname</t>
-  </si>
-  <si>
     <t>Style Details</t>
   </si>
   <si>
@@ -236,13 +197,75 @@
   </si>
   <si>
     <t>Munirr</t>
+  </si>
+  <si>
+    <t>CC-SampleLayout6</t>
+  </si>
+  <si>
+    <t>CC-SampleLayout6 Longname</t>
+  </si>
+  <si>
+    <t>cc-</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dear &lt;comms-data&gt;$Data{"Id":"ownerFirstName"}&lt;/comms-data&gt;,
+                    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Welcome to Automation Testing!!</t>
+    </r>
+  </si>
+  <si>
+    <t>muni1</t>
+  </si>
+  <si>
+    <t>msingiri</t>
+  </si>
+  <si>
+    <t>ccs-auto4-</t>
+  </si>
+  <si>
+    <t>ccs-auto3-</t>
+  </si>
+  <si>
+    <t>CC-StyleLongname1</t>
+  </si>
+  <si>
+    <t>CC-StyleDescription</t>
+  </si>
+  <si>
+    <t>CC-AutoStyleName1</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Attribute details</t>
+  </si>
+  <si>
+    <t>Calibri</t>
+  </si>
+  <si>
+    <t>Font-family</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +277,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -314,12 +345,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -341,6 +398,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -650,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,10 +734,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -787,20 +851,20 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -832,59 +896,59 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="H2" s="4">
-        <v>44042</v>
+        <v>44105</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="H3" s="4">
-        <v>44042</v>
+        <v>44105</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>17</v>
@@ -896,6 +960,7 @@
     <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -921,19 +986,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -947,25 +1012,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H2" s="4">
         <v>44042</v>
@@ -973,25 +1038,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H3" s="4">
         <v>44042</v>
@@ -1010,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,93 +1098,93 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="G1" s="11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="N2" s="12"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H3" s="3">
         <v>8.5</v>
@@ -1128,19 +1193,19 @@
         <v>11</v>
       </c>
       <c r="J3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1160,22 +1225,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,69 +1238,138 @@
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="10" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>64</v>
+      <c r="G3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>